<commit_message>
ADD all labs xlsx and docx
</commit_message>
<xml_diff>
--- a/sem2/MCH/lab1.02/Data.xlsx
+++ b/sem2/MCH/lab1.02/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyaa/iDevelop/itmo-uni/sem2/MCH/lab1.02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilyaa/dev/itmo-uni/sem2/MCH/lab1.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B47DF6-6300-AD4A-B19A-A90DD197BBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662E6C04-97DC-C147-9F83-9B8E3118AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{4AAE61A7-0FF2-C54B-9335-56428A875E03}"/>
   </bookViews>
@@ -1012,6 +1012,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1027,13 +1034,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2343,19 +2343,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.9743589743589737E-3</c:v>
+                  <c:v>-8.9743589743589737E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1794871794871797E-2</c:v>
+                  <c:v>-2.1794871794871797E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3333333333333333E-2</c:v>
+                  <c:v>-3.3333333333333333E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3589743589743594E-2</c:v>
+                  <c:v>-4.3589743589743594E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6410256410256404E-2</c:v>
+                  <c:v>-5.6410256410256404E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5314,8 +5314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E08DD0-596B-3341-91E4-14AB8D2C3883}">
   <dimension ref="A1:AM105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="124" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5360,19 +5360,19 @@
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:39" ht="17" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="19" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="15"/>
       <c r="N3" t="s">
         <v>14</v>
@@ -5436,7 +5436,7 @@
       </c>
     </row>
     <row r="4" spans="1:39" ht="17" thickBot="1">
-      <c r="A4" s="18"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -5467,13 +5467,13 @@
       <c r="K4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="19">
         <v>1</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="19">
         <v>186</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="19">
         <v>177</v>
       </c>
       <c r="Q4">
@@ -5504,8 +5504,8 @@
         <v>1</v>
       </c>
       <c r="Z4" s="8">
-        <f>-(($P$34-O4)-($Q$34-P4))/1000/($O$34-$N$34)</f>
-        <v>8.9743589743589737E-3</v>
+        <f>(($P$34-O4)-($Q$34-P4))/1000/($O$34-$N$34)</f>
+        <v>-8.9743589743589737E-3</v>
       </c>
       <c r="AA4" t="s">
         <v>64</v>
@@ -5518,11 +5518,11 @@
       </c>
       <c r="AD4">
         <f>Z4*AC4</f>
-        <v>9.8691630949695889E-4</v>
+        <v>-9.8691630949695889E-4</v>
       </c>
       <c r="AE4">
         <f>(SUM(AD4:AD8)-1/5*SUM(AC4:AC8)*SUM(Z4:Z8))/(SUM(AD10:AD14)-1/5*(SUM(Z4:Z8)^2))</f>
-        <v>9.2482723855671907</v>
+        <v>-9.2482723855671907</v>
       </c>
       <c r="AF4">
         <f>1/5*(SUM(AC4:AC8)-AE4*SUM(Z4:Z8))</f>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="AK4" s="13">
         <f>AJ4/AE4</f>
-        <v>5.3697707621554659E-2</v>
+        <v>-5.3697707621554659E-2</v>
       </c>
       <c r="AL4">
         <v>8.9743589743589737E-3</v>
@@ -5596,9 +5596,9 @@
         <f>F5/G5</f>
         <v>0.10964912280701755</v>
       </c>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
       <c r="Q5">
         <v>2</v>
       </c>
@@ -5623,8 +5623,8 @@
         <v>2</v>
       </c>
       <c r="Z5" s="8">
-        <f>-(($P$34-O9)-($Q$34-P9))/1000/($O$34-$N$34)</f>
-        <v>2.1794871794871797E-2</v>
+        <f>(($P$34-O9)-($Q$34-P9))/1000/($O$34-$N$34)</f>
+        <v>-2.1794871794871797E-2</v>
       </c>
       <c r="AA5" s="8" t="s">
         <v>66</v>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="AD5">
         <f t="shared" ref="AD5:AD8" si="0">Z5*AC5</f>
-        <v>4.5696467931831625E-3</v>
+        <v>-4.5696467931831625E-3</v>
       </c>
       <c r="AG5">
         <f t="shared" ref="AG5:AG7" si="1">AC5-($AF$4+$AE$4*Z5)</f>
@@ -5691,9 +5691,9 @@
         <f t="shared" ref="K6:K9" si="7">F6/G6</f>
         <v>0.11965811965811962</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
       <c r="Q6">
         <v>3</v>
       </c>
@@ -5703,7 +5703,7 @@
       <c r="S6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="T6" s="17" t="s">
         <v>81</v>
       </c>
       <c r="U6" s="8">
@@ -5718,8 +5718,8 @@
         <v>3</v>
       </c>
       <c r="Z6" s="8">
-        <f>-(($P$34-O14)-($Q$34-P14))/1000/($O$34-$N$34)</f>
-        <v>3.3333333333333333E-2</v>
+        <f>(($P$34-O14)-($Q$34-P14))/1000/($O$34-$N$34)</f>
+        <v>-3.3333333333333333E-2</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>68</v>
@@ -5732,7 +5732,7 @@
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>1.1187607573149738E-2</v>
+        <v>-1.1187607573149738E-2</v>
       </c>
       <c r="AG6">
         <f t="shared" si="1"/>
@@ -5775,7 +5775,7 @@
         <v>2.3099999999999996</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" ref="I6:I9" si="8">F7^2</f>
+        <f t="shared" ref="I7:I9" si="8">F7^2</f>
         <v>0.30249999999999994</v>
       </c>
       <c r="J7">
@@ -5786,9 +5786,9 @@
         <f t="shared" si="7"/>
         <v>0.13095238095238093</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
       <c r="Q7">
         <v>4</v>
       </c>
@@ -5798,7 +5798,7 @@
       <c r="S7">
         <v>4</v>
       </c>
-      <c r="T7" s="24" t="s">
+      <c r="T7" s="18" t="s">
         <v>82</v>
       </c>
       <c r="U7" s="8">
@@ -5813,8 +5813,8 @@
         <v>4</v>
       </c>
       <c r="Z7" s="8">
-        <f>-(($P$34-O19)-($Q$34-P19))/1000/($O$34-$N$34)</f>
-        <v>4.3589743589743594E-2</v>
+        <f>(($P$34-O19)-($Q$34-P19))/1000/($O$34-$N$34)</f>
+        <v>-4.3589743589743594E-2</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>70</v>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>1.8609742747673793E-2</v>
+        <v>-1.8609742747673793E-2</v>
       </c>
       <c r="AG7">
         <f t="shared" si="1"/>
@@ -5881,9 +5881,9 @@
         <f t="shared" si="7"/>
         <v>0.10101010101010101</v>
       </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
       <c r="Q8">
         <v>5</v>
       </c>
@@ -5893,7 +5893,7 @@
       <c r="S8">
         <v>4.2</v>
       </c>
-      <c r="T8" s="24" t="s">
+      <c r="T8" s="18" t="s">
         <v>83</v>
       </c>
       <c r="U8" s="13">
@@ -5910,8 +5910,8 @@
         <v>5</v>
       </c>
       <c r="Z8" s="8">
-        <f>-(($P$34-O24)-($Q$34-P24))/1000/($O$34-$N$34)</f>
-        <v>5.6410256410256404E-2</v>
+        <f>(($P$34-O24)-($Q$34-P24))/1000/($O$34-$N$34)</f>
+        <v>-5.6410256410256404E-2</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>72</v>
@@ -5924,7 +5924,7 @@
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>3.053435114503817E-2</v>
+        <v>-3.053435114503817E-2</v>
       </c>
       <c r="AG8">
         <f>AC8-($AF$4+$AE$4*Z8)</f>
@@ -5978,13 +5978,13 @@
         <f t="shared" si="7"/>
         <v>9.8958333333333356E-2</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="19">
         <v>2</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="19">
         <v>196</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="19">
         <v>177</v>
       </c>
       <c r="Q9">
@@ -6045,9 +6045,9 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
       <c r="Q10">
         <v>2</v>
       </c>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="AJ10">
         <f>ABS(AJ9-AE4)</f>
-        <v>0.57122761443280901</v>
+        <v>19.067772385567189</v>
       </c>
     </row>
     <row r="11" spans="1:39" ht="17">
@@ -6126,9 +6126,9 @@
         <f>$B$19*F5</f>
         <v>2.380601792573624</v>
       </c>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
       <c r="Q11">
         <v>3</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="S11">
         <v>3.1</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="T11" s="17" t="s">
         <v>81</v>
       </c>
       <c r="U11" s="8">
@@ -6185,9 +6185,9 @@
         <f t="shared" ref="I12:I15" si="12">$B$19*F6</f>
         <v>3.3328425096030734</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
       <c r="Q12">
         <v>4</v>
       </c>
@@ -6197,7 +6197,7 @@
       <c r="S12">
         <v>3</v>
       </c>
-      <c r="T12" s="24" t="s">
+      <c r="T12" s="18" t="s">
         <v>82</v>
       </c>
       <c r="U12" s="8">
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="17">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="8">
@@ -6244,9 +6244,9 @@
         <f t="shared" si="12"/>
         <v>5.2373239436619725</v>
       </c>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
       <c r="Q13">
         <v>5</v>
       </c>
@@ -6256,7 +6256,7 @@
       <c r="S13">
         <v>3</v>
       </c>
-      <c r="T13" s="24" t="s">
+      <c r="T13" s="18" t="s">
         <v>83</v>
       </c>
       <c r="U13" s="13">
@@ -6290,7 +6290,7 @@
       </c>
     </row>
     <row r="14" spans="1:39">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="8">
@@ -6322,13 +6322,13 @@
         <f t="shared" si="12"/>
         <v>7.1418053777208721</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="19">
         <v>3</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="19">
         <v>205</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="19">
         <v>177</v>
       </c>
       <c r="Q14">
@@ -6375,7 +6375,7 @@
       </c>
     </row>
     <row r="15" spans="1:39">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B15" s="13">
@@ -6406,9 +6406,9 @@
         <f t="shared" si="12"/>
         <v>9.0462868117797726</v>
       </c>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
       <c r="Q15">
         <v>2</v>
       </c>
@@ -6463,9 +6463,9 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
       <c r="Q16">
         <v>3</v>
       </c>
@@ -6475,7 +6475,7 @@
       <c r="S16">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T16" s="23" t="s">
+      <c r="T16" s="17" t="s">
         <v>81</v>
       </c>
       <c r="U16" s="8">
@@ -6523,9 +6523,9 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
       <c r="Q17">
         <v>4</v>
       </c>
@@ -6535,7 +6535,7 @@
       <c r="S17">
         <v>2.4</v>
       </c>
-      <c r="T17" s="24" t="s">
+      <c r="T17" s="18" t="s">
         <v>82</v>
       </c>
       <c r="U17" s="8">
@@ -6583,9 +6583,9 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
       <c r="Q18">
         <v>5</v>
       </c>
@@ -6595,7 +6595,7 @@
       <c r="S18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="T18" s="24" t="s">
+      <c r="T18" s="18" t="s">
         <v>83</v>
       </c>
       <c r="U18" s="13">
@@ -6647,13 +6647,13 @@
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
-      <c r="N19" s="16">
+      <c r="N19" s="19">
         <v>4</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="19">
         <v>214</v>
       </c>
-      <c r="P19" s="16">
+      <c r="P19" s="19">
         <v>178</v>
       </c>
       <c r="Q19">
@@ -6705,9 +6705,9 @@
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
       <c r="Q20">
         <v>2</v>
       </c>
@@ -6763,9 +6763,9 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
       <c r="Q21">
         <v>3</v>
       </c>
@@ -6775,7 +6775,7 @@
       <c r="S21">
         <v>2.1</v>
       </c>
-      <c r="T21" s="23" t="s">
+      <c r="T21" s="17" t="s">
         <v>81</v>
       </c>
       <c r="U21" s="8">
@@ -6821,9 +6821,9 @@
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
       <c r="Q22">
         <v>4</v>
       </c>
@@ -6833,7 +6833,7 @@
       <c r="S22">
         <v>2.1</v>
       </c>
-      <c r="T22" s="24" t="s">
+      <c r="T22" s="18" t="s">
         <v>82</v>
       </c>
       <c r="U22" s="8">
@@ -6850,7 +6850,7 @@
       <c r="Y22">
         <v>9.5296822845488682E-2</v>
       </c>
-      <c r="Z22" s="22" t="s">
+      <c r="Z22" s="16" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6873,9 +6873,9 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
       <c r="Q23">
         <v>5</v>
       </c>
@@ -6885,7 +6885,7 @@
       <c r="S23">
         <v>2.1</v>
       </c>
-      <c r="T23" s="24" t="s">
+      <c r="T23" s="18" t="s">
         <v>83</v>
       </c>
       <c r="U23" s="13">
@@ -6903,7 +6903,7 @@
       <c r="Y23">
         <v>8.6809011308990561E-2</v>
       </c>
-      <c r="Z23" s="22" t="s">
+      <c r="Z23" s="16" t="s">
         <v>76</v>
       </c>
     </row>
@@ -6922,13 +6922,13 @@
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="16">
+      <c r="N24" s="19">
         <v>5</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="19">
         <v>224</v>
       </c>
-      <c r="P24" s="16">
+      <c r="P24" s="19">
         <v>178</v>
       </c>
       <c r="Q24">
@@ -6976,9 +6976,9 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
       <c r="Q25">
         <v>2</v>
       </c>
@@ -6999,14 +6999,14 @@
         <f>SQRT(SUM(T52:T56)/20)</f>
         <v>2.4494897427831747E-2</v>
       </c>
-      <c r="Z25" s="22" t="s">
+      <c r="Z25" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:27" ht="17">
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
       <c r="Q26">
         <v>3</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="S26">
         <v>1.9</v>
       </c>
-      <c r="T26" s="23" t="s">
+      <c r="T26" s="17" t="s">
         <v>81</v>
       </c>
       <c r="U26" s="8">
@@ -7029,9 +7029,9 @@
       </c>
     </row>
     <row r="27" spans="1:27">
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
       <c r="Q27">
         <v>4</v>
       </c>
@@ -7041,7 +7041,7 @@
       <c r="S27">
         <v>1.8</v>
       </c>
-      <c r="T27" s="24" t="s">
+      <c r="T27" s="18" t="s">
         <v>82</v>
       </c>
       <c r="U27" s="8">
@@ -7054,9 +7054,9 @@
       </c>
     </row>
     <row r="28" spans="1:27">
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
       <c r="Q28">
         <v>5</v>
       </c>
@@ -7066,7 +7066,7 @@
       <c r="S28">
         <v>1.9</v>
       </c>
-      <c r="T28" s="24" t="s">
+      <c r="T28" s="18" t="s">
         <v>83</v>
       </c>
       <c r="U28" s="13">
@@ -7755,24 +7755,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N19:N23"/>
+    <mergeCell ref="O19:O23"/>
+    <mergeCell ref="P19:P23"/>
+    <mergeCell ref="N24:N28"/>
+    <mergeCell ref="O24:O28"/>
+    <mergeCell ref="P24:P28"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="N14:N18"/>
+    <mergeCell ref="O14:O18"/>
+    <mergeCell ref="P14:P18"/>
     <mergeCell ref="N4:N8"/>
     <mergeCell ref="O4:O8"/>
     <mergeCell ref="P4:P8"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="N14:N18"/>
-    <mergeCell ref="O14:O18"/>
-    <mergeCell ref="P14:P18"/>
-    <mergeCell ref="N19:N23"/>
-    <mergeCell ref="O19:O23"/>
-    <mergeCell ref="P19:P23"/>
-    <mergeCell ref="N24:N28"/>
-    <mergeCell ref="O24:O28"/>
-    <mergeCell ref="P24:P28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>